<commit_message>
adding revised diagnoses outcomes
</commit_message>
<xml_diff>
--- a/applications/SHIELD/Documentation/Syphilis Manager Data Overview_4.8.25.xlsx
+++ b/applications/SHIELD/Documentation/Syphilis Manager Data Overview_4.8.25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/pkasaie1_jh_edu/Documents/SHIELDR01/SHIELD-Shared/Data Manager Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/pkasaie1_jh_edu/Documents/SHIELDR01/Simulation/code/jheem_analyses/applications/SHIELD/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1074" documentId="13_ncr:1_{460D6CD4-A812-4C2E-A51F-0C846BEEF02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D4E2402-2748-4B8D-A99F-44E1CC038AFD}"/>
   <bookViews>
-    <workbookView xWindow="75500" yWindow="500" windowWidth="38080" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="74120" yWindow="500" windowWidth="34560" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -930,7 +930,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1133,11 +1133,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1450,28 +1450,28 @@
   <dimension ref="A1:M115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="F9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="28.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="44.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="33.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="22.5" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="67.7109375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="42.7109375" customWidth="1"/>
+    <col min="10" max="10" width="33.5" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="67.6640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="65.099999999999994" thickBot="1">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="33" thickTop="1">
+    <row r="2" spans="1:13" ht="33" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="12" t="s">
         <v>13</v>
@@ -1548,7 +1548,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="48">
+    <row r="3" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>13</v>
@@ -1584,7 +1584,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="32.1">
+    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>13</v>
@@ -1620,7 +1620,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="32.1">
+    <row r="5" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="12" t="s">
         <v>13</v>
@@ -1656,7 +1656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.95">
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="12" t="s">
         <v>13</v>
@@ -1689,7 +1689,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30.95" customHeight="1">
+    <row r="7" spans="1:13" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
       <c r="B7" s="12" t="s">
         <v>13</v>
@@ -1728,7 +1728,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.95">
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="12" t="s">
         <v>13</v>
@@ -1767,7 +1767,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.95">
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="12" t="s">
         <v>13</v>
@@ -1800,7 +1800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="63.95">
+    <row r="10" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="12" t="s">
         <v>13</v>
@@ -1836,7 +1836,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
         <v>13</v>
@@ -1872,7 +1872,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.95">
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="12" t="s">
         <v>13</v>
@@ -1905,7 +1905,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="32.1">
+    <row r="13" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="12" t="s">
         <v>13</v>
@@ -1941,7 +1941,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="32.1">
+    <row r="14" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="12" t="s">
         <v>13</v>
@@ -1977,7 +1977,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.95">
+    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="12" t="s">
         <v>13</v>
@@ -2013,7 +2013,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.95">
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="12" t="s">
         <v>13</v>
@@ -2046,7 +2046,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="32.1">
+    <row r="17" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="12" t="s">
         <v>13</v>
@@ -2082,7 +2082,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="48">
+    <row r="18" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="12" t="s">
         <v>13</v>
@@ -2118,7 +2118,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="32.1">
+    <row r="19" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="12" t="s">
         <v>13</v>
@@ -2154,7 +2154,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="32.1">
+    <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>60</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.95">
+    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="12" t="s">
         <v>13</v>
@@ -2225,7 +2225,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.95">
+    <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="12" t="s">
         <v>13</v>
@@ -2258,7 +2258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="32.1">
+    <row r="23" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="12" t="s">
         <v>13</v>
@@ -2294,7 +2294,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="32.1">
+    <row r="24" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="12" t="s">
         <v>13</v>
@@ -2324,7 +2324,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="32.1">
+    <row r="25" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="12" t="s">
         <v>13</v>
@@ -2360,7 +2360,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.95">
+    <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="12" t="s">
         <v>13</v>
@@ -2390,7 +2390,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.95">
+    <row r="27" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="12" t="s">
         <v>13</v>
@@ -2420,7 +2420,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.95">
+    <row r="28" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="12" t="s">
         <v>13</v>
@@ -2459,7 +2459,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="32.1">
+    <row r="29" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="12" t="s">
         <v>13</v>
@@ -2495,7 +2495,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="32.1">
+    <row r="30" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="12" t="s">
         <v>13</v>
@@ -2531,7 +2531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="32.1">
+    <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
         <v>13</v>
@@ -2567,7 +2567,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15.95">
+    <row r="32" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="12" t="s">
         <v>13</v>
@@ -2600,8 +2600,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="16" customFormat="1" ht="15.95">
-      <c r="A33" s="28" t="s">
+    <row r="33" spans="1:13" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="32" t="s">
         <v>83</v>
       </c>
       <c r="B33" s="15" t="s">
@@ -2639,8 +2639,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="16" customFormat="1" ht="15.95">
-      <c r="A34" s="28"/>
+    <row r="34" spans="1:13" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="32"/>
       <c r="B34" s="15" t="s">
         <v>84</v>
       </c>
@@ -2676,8 +2676,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="16" customFormat="1" ht="15.95">
-      <c r="A35" s="28"/>
+    <row r="35" spans="1:13" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="32"/>
       <c r="B35" s="15" t="s">
         <v>84</v>
       </c>
@@ -2713,8 +2713,8 @@
       </c>
       <c r="M35" s="13"/>
     </row>
-    <row r="36" spans="1:13" s="16" customFormat="1" ht="63.95">
-      <c r="A36" s="28"/>
+    <row r="36" spans="1:13" s="16" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A36" s="32"/>
       <c r="B36" s="15" t="s">
         <v>84</v>
       </c>
@@ -2750,8 +2750,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="63.95">
-      <c r="A37" s="28"/>
+    <row r="37" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A37" s="32"/>
       <c r="B37" s="15" t="s">
         <v>84</v>
       </c>
@@ -2787,8 +2787,8 @@
       </c>
       <c r="M37" s="13"/>
     </row>
-    <row r="38" spans="1:13" s="16" customFormat="1" ht="15.95">
-      <c r="A38" s="28"/>
+    <row r="38" spans="1:13" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="32"/>
       <c r="B38" s="15" t="s">
         <v>84</v>
       </c>
@@ -2822,8 +2822,8 @@
       <c r="L38" s="14"/>
       <c r="M38" s="13"/>
     </row>
-    <row r="39" spans="1:13" ht="15.95">
-      <c r="A39" s="28"/>
+    <row r="39" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="32"/>
       <c r="B39" s="15" t="s">
         <v>84</v>
       </c>
@@ -2859,8 +2859,8 @@
       </c>
       <c r="M39" s="13"/>
     </row>
-    <row r="40" spans="1:13" ht="15.95">
-      <c r="A40" s="28"/>
+    <row r="40" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="32"/>
       <c r="B40" s="15" t="s">
         <v>84</v>
       </c>
@@ -2894,8 +2894,8 @@
       <c r="L40" s="14"/>
       <c r="M40" s="13"/>
     </row>
-    <row r="41" spans="1:13" ht="15.95">
-      <c r="A41" s="28"/>
+    <row r="41" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="32"/>
       <c r="B41" s="15" t="s">
         <v>84</v>
       </c>
@@ -2929,8 +2929,8 @@
       <c r="L41" s="14"/>
       <c r="M41" s="13"/>
     </row>
-    <row r="42" spans="1:13" ht="63.95">
-      <c r="A42" s="28"/>
+    <row r="42" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A42" s="32"/>
       <c r="B42" s="15" t="s">
         <v>84</v>
       </c>
@@ -2964,8 +2964,8 @@
       <c r="L42" s="14"/>
       <c r="M42" s="13"/>
     </row>
-    <row r="43" spans="1:13" ht="15.95">
-      <c r="A43" s="28"/>
+    <row r="43" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="32"/>
       <c r="B43" s="15" t="s">
         <v>84</v>
       </c>
@@ -3001,8 +3001,8 @@
       </c>
       <c r="M43" s="13"/>
     </row>
-    <row r="44" spans="1:13" ht="15.95">
-      <c r="A44" s="28"/>
+    <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="32"/>
       <c r="B44" s="15" t="s">
         <v>84</v>
       </c>
@@ -3034,8 +3034,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="15.95">
-      <c r="A45" s="28"/>
+    <row r="45" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="32"/>
       <c r="B45" s="15" t="s">
         <v>84</v>
       </c>
@@ -3067,8 +3067,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="15.95">
-      <c r="A46" s="28"/>
+    <row r="46" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="32"/>
       <c r="B46" s="15" t="s">
         <v>84</v>
       </c>
@@ -3100,8 +3100,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="15.95">
-      <c r="A47" s="28"/>
+    <row r="47" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="32"/>
       <c r="B47" s="15" t="s">
         <v>84</v>
       </c>
@@ -3133,8 +3133,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="48">
-      <c r="A48" s="28"/>
+    <row r="48" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A48" s="32"/>
       <c r="B48" s="15" t="s">
         <v>84</v>
       </c>
@@ -3166,8 +3166,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="15.95">
-      <c r="A49" s="28"/>
+    <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="32"/>
       <c r="B49" s="15" t="s">
         <v>84</v>
       </c>
@@ -3199,8 +3199,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="48">
-      <c r="A50" s="28"/>
+    <row r="50" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A50" s="32"/>
       <c r="B50" s="15" t="s">
         <v>84</v>
       </c>
@@ -3232,8 +3232,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="32.1">
-      <c r="A51" s="28"/>
+    <row r="51" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A51" s="32"/>
       <c r="B51" s="15" t="s">
         <v>84</v>
       </c>
@@ -3268,8 +3268,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="48">
-      <c r="A52" s="28"/>
+    <row r="52" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A52" s="32"/>
       <c r="B52" s="15" t="s">
         <v>84</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="15.95">
+    <row r="53" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="29" t="s">
         <v>124</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="15.95">
+    <row r="54" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="29"/>
       <c r="B54" s="17" t="s">
         <v>125</v>
@@ -3381,7 +3381,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15.95">
+    <row r="55" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="29"/>
       <c r="B55" s="17" t="s">
         <v>125</v>
@@ -3414,7 +3414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.95">
+    <row r="56" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="29"/>
       <c r="B56" s="17" t="s">
         <v>125</v>
@@ -3447,7 +3447,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="15.95">
+    <row r="57" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="29"/>
       <c r="B57" s="17" t="s">
         <v>125</v>
@@ -3483,7 +3483,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="15.95">
+    <row r="58" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="29"/>
       <c r="B58" s="17" t="s">
         <v>125</v>
@@ -3519,7 +3519,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="15.95">
+    <row r="59" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="29"/>
       <c r="B59" s="17" t="s">
         <v>125</v>
@@ -3555,7 +3555,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="15.95">
+    <row r="60" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="29"/>
       <c r="B60" s="17" t="s">
         <v>125</v>
@@ -3585,7 +3585,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="15.95">
+    <row r="61" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="29"/>
       <c r="B61" s="17" t="s">
         <v>125</v>
@@ -3618,7 +3618,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="15.95">
+    <row r="62" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="29"/>
       <c r="B62" s="17" t="s">
         <v>125</v>
@@ -3654,7 +3654,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="15.95">
+    <row r="63" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="29"/>
       <c r="B63" s="17" t="s">
         <v>125</v>
@@ -3690,7 +3690,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="15.95">
+    <row r="64" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="29"/>
       <c r="B64" s="17" t="s">
         <v>125</v>
@@ -3723,7 +3723,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="15.95">
+    <row r="65" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="29"/>
       <c r="B65" s="17" t="s">
         <v>125</v>
@@ -3756,7 +3756,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="15.95">
+    <row r="66" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="29"/>
       <c r="B66" s="17" t="s">
         <v>125</v>
@@ -3792,7 +3792,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="15.95">
+    <row r="67" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="29"/>
       <c r="B67" s="17" t="s">
         <v>125</v>
@@ -3825,7 +3825,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="15.95">
+    <row r="68" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="29"/>
       <c r="B68" s="18" t="s">
         <v>158</v>
@@ -3864,7 +3864,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="15.95">
+    <row r="69" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="29"/>
       <c r="B69" s="18" t="s">
         <v>158</v>
@@ -3903,7 +3903,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="13" customFormat="1" ht="32.1">
+    <row r="70" spans="1:13" s="13" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="29"/>
       <c r="B70" s="18" t="s">
         <v>158</v>
@@ -3939,7 +3939,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="13" customFormat="1" ht="15.95">
+    <row r="71" spans="1:13" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="29"/>
       <c r="B71" s="18" t="s">
         <v>158</v>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="L71" s="14"/>
     </row>
-    <row r="72" spans="1:13" s="13" customFormat="1" ht="32.1">
+    <row r="72" spans="1:13" s="13" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="29"/>
       <c r="B72" s="18" t="s">
         <v>158</v>
@@ -4009,7 +4009,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="13" customFormat="1" ht="15.95">
+    <row r="73" spans="1:13" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="29"/>
       <c r="B73" s="18" t="s">
         <v>158</v>
@@ -4043,8 +4043,8 @@
       </c>
       <c r="L73" s="14"/>
     </row>
-    <row r="74" spans="1:13" ht="48">
-      <c r="A74" s="28" t="s">
+    <row r="74" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A74" s="32" t="s">
         <v>178</v>
       </c>
       <c r="B74" s="15" t="s">
@@ -4084,8 +4084,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="32.1">
-      <c r="A75" s="28"/>
+    <row r="75" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A75" s="32"/>
       <c r="B75" s="15" t="s">
         <v>84</v>
       </c>
@@ -4123,8 +4123,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="63.95">
-      <c r="A76" s="28"/>
+    <row r="76" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A76" s="32"/>
       <c r="B76" s="15" t="s">
         <v>84</v>
       </c>
@@ -4156,8 +4156,8 @@
         <v>194</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="32.1">
-      <c r="A77" s="28"/>
+    <row r="77" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A77" s="32"/>
       <c r="B77" s="15" t="s">
         <v>84</v>
       </c>
@@ -4192,8 +4192,8 @@
         <v>197</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="80.099999999999994">
-      <c r="A78" s="28"/>
+    <row r="78" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+      <c r="A78" s="32"/>
       <c r="B78" s="15" t="s">
         <v>84</v>
       </c>
@@ -4231,8 +4231,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="80.099999999999994">
-      <c r="A79" s="28"/>
+    <row r="79" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+      <c r="A79" s="32"/>
       <c r="B79" s="15" t="s">
         <v>84</v>
       </c>
@@ -4270,8 +4270,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="80.099999999999994">
-      <c r="A80" s="28"/>
+    <row r="80" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+      <c r="A80" s="32"/>
       <c r="B80" s="15" t="s">
         <v>84</v>
       </c>
@@ -4309,8 +4309,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="80.099999999999994">
-      <c r="A81" s="28"/>
+    <row r="81" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+      <c r="A81" s="32"/>
       <c r="B81" s="15" t="s">
         <v>84</v>
       </c>
@@ -4348,8 +4348,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="111.95">
-      <c r="A82" s="28"/>
+    <row r="82" spans="1:13" ht="112" x14ac:dyDescent="0.2">
+      <c r="A82" s="32"/>
       <c r="B82" s="15" t="s">
         <v>84</v>
       </c>
@@ -4387,8 +4387,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="111.95">
-      <c r="A83" s="28"/>
+    <row r="83" spans="1:13" ht="112" x14ac:dyDescent="0.2">
+      <c r="A83" s="32"/>
       <c r="B83" s="15" t="s">
         <v>84</v>
       </c>
@@ -4426,8 +4426,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="111.95">
-      <c r="A84" s="28"/>
+    <row r="84" spans="1:13" ht="112" x14ac:dyDescent="0.2">
+      <c r="A84" s="32"/>
       <c r="B84" s="15" t="s">
         <v>84</v>
       </c>
@@ -4465,8 +4465,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="111.95">
-      <c r="A85" s="28"/>
+    <row r="85" spans="1:13" ht="112" x14ac:dyDescent="0.2">
+      <c r="A85" s="32"/>
       <c r="B85" s="15" t="s">
         <v>84</v>
       </c>
@@ -4504,8 +4504,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="46.5" customHeight="1">
-      <c r="A86" s="28"/>
+    <row r="86" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="32"/>
       <c r="B86" s="15" t="s">
         <v>84</v>
       </c>
@@ -4540,8 +4540,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="46.5" customHeight="1">
-      <c r="A87" s="28"/>
+    <row r="87" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="32"/>
       <c r="B87" s="15" t="s">
         <v>84</v>
       </c>
@@ -4576,8 +4576,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="86.25" customHeight="1">
-      <c r="A88" s="28"/>
+    <row r="88" spans="1:13" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="32"/>
       <c r="B88" s="15" t="s">
         <v>84</v>
       </c>
@@ -4612,8 +4612,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="86.25" customHeight="1">
-      <c r="A89" s="28"/>
+    <row r="89" spans="1:13" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="32"/>
       <c r="B89" s="15" t="s">
         <v>84</v>
       </c>
@@ -4645,8 +4645,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="80.099999999999994">
-      <c r="A90" s="28"/>
+    <row r="90" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+      <c r="A90" s="32"/>
       <c r="B90" s="15" t="s">
         <v>84</v>
       </c>
@@ -4681,8 +4681,8 @@
         <v>218</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="32.1">
-      <c r="A91" s="30" t="s">
+    <row r="91" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A91" s="28" t="s">
         <v>219</v>
       </c>
       <c r="B91" s="20" t="s">
@@ -4719,8 +4719,8 @@
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="48">
-      <c r="A92" s="30"/>
+    <row r="92" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A92" s="28"/>
       <c r="B92" s="20" t="s">
         <v>220</v>
       </c>
@@ -4755,8 +4755,8 @@
         <v>224</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="15.95">
-      <c r="A93" s="30"/>
+    <row r="93" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="28"/>
       <c r="B93" s="20" t="s">
         <v>220</v>
       </c>
@@ -4791,8 +4791,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="15.95">
-      <c r="A94" s="30"/>
+    <row r="94" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="28"/>
       <c r="B94" s="20" t="s">
         <v>220</v>
       </c>
@@ -4827,9 +4827,9 @@
         <v>228</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15.95" thickBot="1"/>
-    <row r="98" spans="1:12" ht="17.100000000000001" thickTop="1">
-      <c r="A98" s="31" t="s">
+    <row r="97" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="30" t="s">
         <v>229</v>
       </c>
       <c r="B98" s="17" t="s">
@@ -4866,8 +4866,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.95">
-      <c r="A99" s="32"/>
+    <row r="99" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="31"/>
       <c r="B99" s="17" t="s">
         <v>125</v>
       </c>
@@ -4899,8 +4899,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.95">
-      <c r="A100" s="32"/>
+    <row r="100" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="31"/>
       <c r="B100" s="17" t="s">
         <v>125</v>
       </c>
@@ -4932,8 +4932,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.95">
-      <c r="A101" s="32"/>
+    <row r="101" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="31"/>
       <c r="B101" s="17" t="s">
         <v>125</v>
       </c>
@@ -4965,8 +4965,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="32.1">
-      <c r="A102" s="32"/>
+    <row r="102" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A102" s="31"/>
       <c r="B102" s="17" t="s">
         <v>125</v>
       </c>
@@ -5001,8 +5001,8 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15.95">
-      <c r="A103" s="32"/>
+    <row r="103" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="31"/>
       <c r="B103" s="17" t="s">
         <v>125</v>
       </c>
@@ -5037,8 +5037,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15.95">
-      <c r="A104" s="32"/>
+    <row r="104" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A104" s="31"/>
       <c r="B104" s="17" t="s">
         <v>125</v>
       </c>
@@ -5073,8 +5073,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.95">
-      <c r="A105" s="32"/>
+    <row r="105" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="31"/>
       <c r="B105" s="17" t="s">
         <v>125</v>
       </c>
@@ -5109,8 +5109,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15.95">
-      <c r="A106" s="32"/>
+    <row r="106" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A106" s="31"/>
       <c r="B106" s="17" t="s">
         <v>125</v>
       </c>
@@ -5145,8 +5145,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="32.1">
-      <c r="A107" s="32"/>
+    <row r="107" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A107" s="31"/>
       <c r="B107" s="17" t="s">
         <v>125</v>
       </c>
@@ -5181,8 +5181,8 @@
         <v>249</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="32.1">
-      <c r="A108" s="32"/>
+    <row r="108" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A108" s="31"/>
       <c r="B108" s="17" t="s">
         <v>125</v>
       </c>
@@ -5217,8 +5217,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="32.1">
-      <c r="A109" s="32"/>
+    <row r="109" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A109" s="31"/>
       <c r="B109" s="17" t="s">
         <v>125</v>
       </c>
@@ -5253,8 +5253,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="32.1">
-      <c r="A110" s="32"/>
+    <row r="110" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A110" s="31"/>
       <c r="B110" s="17" t="s">
         <v>125</v>
       </c>
@@ -5289,8 +5289,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="32.1">
-      <c r="A111" s="32"/>
+    <row r="111" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A111" s="31"/>
       <c r="B111" s="17" t="s">
         <v>125</v>
       </c>
@@ -5325,8 +5325,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="32.1">
-      <c r="A112" s="32"/>
+    <row r="112" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A112" s="31"/>
       <c r="B112" s="17" t="s">
         <v>125</v>
       </c>
@@ -5361,8 +5361,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="32.1">
-      <c r="A113" s="32"/>
+    <row r="113" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A113" s="31"/>
       <c r="B113" s="17" t="s">
         <v>125</v>
       </c>
@@ -5397,8 +5397,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="32.1">
-      <c r="A114" s="32"/>
+    <row r="114" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A114" s="31"/>
       <c r="B114" s="17" t="s">
         <v>125</v>
       </c>
@@ -5433,8 +5433,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="32.1">
-      <c r="A115" s="32"/>
+    <row r="115" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A115" s="31"/>
       <c r="B115" s="17" t="s">
         <v>125</v>
       </c>
@@ -5498,16 +5498,16 @@
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" customWidth="1"/>
+    <col min="2" max="2" width="50.5" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="71.7109375" customWidth="1"/>
+    <col min="4" max="4" width="48.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="71.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="33" thickBot="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>255</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.100000000000001" thickTop="1">
+    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32.1">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>232</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32.1">
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.95">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.95">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.95">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.95">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>147</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.95">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>275</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="48">
+    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="48">
+    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>154</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="48">
+    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>153</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="48">
+    <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="48">
+    <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -5745,7 +5745,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="48">
+    <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.95">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>183</v>
       </c>
@@ -5779,22 +5779,22 @@
         <v>282</v>
       </c>
     </row>
-    <row r="20" spans="3:4">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:4">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="3:4">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="3:4">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
     </row>
-    <row r="26" spans="3:4">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C26" s="1"/>
     </row>
-    <row r="28" spans="3:4">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D28" s="6"/>
     </row>
   </sheetData>
@@ -5811,13 +5811,13 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" customWidth="1"/>
-    <col min="2" max="2" width="63.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="46.5" customWidth="1"/>
+    <col min="2" max="2" width="63.83203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="15.95">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>283</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="48">
+    <row r="2" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>285</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="63.95">
+    <row r="3" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="111.95">
+    <row r="4" spans="1:2" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
cleanup missing the proportion.births.congenital. output
</commit_message>
<xml_diff>
--- a/applications/SHIELD/Documentation/Syphilis Manager Data Overview_4.8.25.xlsx
+++ b/applications/SHIELD/Documentation/Syphilis Manager Data Overview_4.8.25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/pkasaie1_jh_edu/Documents/SHIELDR01/Simulation/code/jheem_analyses/applications/SHIELD/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1074" documentId="13_ncr:1_{460D6CD4-A812-4C2E-A51F-0C846BEEF02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D4E2402-2748-4B8D-A99F-44E1CC038AFD}"/>
+  <xr:revisionPtr revIDLastSave="1078" documentId="13_ncr:1_{460D6CD4-A812-4C2E-A51F-0C846BEEF02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B16DA7FE-E96D-984B-A32A-5F867BB9B4CB}"/>
   <bookViews>
-    <workbookView xWindow="74120" yWindow="500" windowWidth="34560" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39560" yWindow="1300" windowWidth="34560" windowHeight="19100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -1450,8 +1450,8 @@
   <dimension ref="A1:M115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
current version post meeting
</commit_message>
<xml_diff>
--- a/applications/SHIELD/Documentation/Syphilis Manager Data Overview_4.8.25.xlsx
+++ b/applications/SHIELD/Documentation/Syphilis Manager Data Overview_4.8.25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/pkasaie1_jh_edu/Documents/SHIELDR01/Simulation/code/jheem_analyses/applications/SHIELD/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1078" documentId="13_ncr:1_{460D6CD4-A812-4C2E-A51F-0C846BEEF02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B16DA7FE-E96D-984B-A32A-5F867BB9B4CB}"/>
+  <xr:revisionPtr revIDLastSave="1080" documentId="13_ncr:1_{460D6CD4-A812-4C2E-A51F-0C846BEEF02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1A3FBCA-9C4B-5A40-AD29-6E01C55B3A80}"/>
   <bookViews>
-    <workbookView xWindow="39560" yWindow="1300" windowWidth="34560" windowHeight="19100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="73740" yWindow="1120" windowWidth="34560" windowHeight="19100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>

</xml_diff>